<commit_message>
Edit book editing feature diagram and description, edit mockup to display save and publish buttons on editChapter and newChapter page
</commit_message>
<xml_diff>
--- a/ressources/project descriptions/Feature description - Book editing management.xlsx
+++ b/ressources/project descriptions/Feature description - Book editing management.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu\Desktop\Fiches descriptives P4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathieu\Desktop\Projet 4 - Aller simple pour l'Alaska\project descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B3BBB663-4B55-4AA6-A2A8-ECF0831F5474}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8B9BD8CB-89D8-4D19-B947-9E3F5767FA95}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1B88FB64-ECA9-408D-A391-F451CFF483CD}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="103">
   <si>
     <t>Numéro</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Performance attendue</t>
   </si>
   <si>
-    <t>L'affichage de l'éditeur doit se faire en moins de 5 secondes.</t>
-  </si>
-  <si>
     <t>Problème non résolus</t>
   </si>
   <si>
@@ -125,72 +122,30 @@
     <t>Il retourne à l'utilisateur un message pour lui signaler que l'enregistrement s'est bien passé.</t>
   </si>
   <si>
-    <t>Il envoie la requête au serveur pour enregistrer le contenu en BDD.</t>
-  </si>
-  <si>
-    <t>Il valide l'édition du chapitre.</t>
-  </si>
-  <si>
-    <t>Il affiche le contenu du chapitre sélectionné par l'utilisateur.</t>
-  </si>
-  <si>
     <t>L'ajout d'un chapitre doit être possible pour l'auteur ainsi que pour l'administrateur.</t>
   </si>
   <si>
     <t>L'utilisateur doit être authentifié en tant qu'auteur ou administrateur.</t>
   </si>
   <si>
-    <t>L'utilisateur a demandé la page 'Ajouter un chapitre' du chapitre en haut de la liste des chapitres déjà existants.</t>
-  </si>
-  <si>
     <t>Il affiche une page d'édition de chapitre vierge.</t>
   </si>
   <si>
-    <t>Il peut décider d'enregistrer un contenu vierge.</t>
-  </si>
-  <si>
     <t>Il peut décider de quitter l'édition d'un nouveau chapitre.</t>
   </si>
   <si>
-    <t>Il peut décider de supprimer le contenu pour repartir sur une nouvelle édition de chapitre.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Il peut décider d'enregistrer le contenu sans rien changer.</t>
-  </si>
-  <si>
-    <t>Il peut décider de quitter l'édition du chapitre.</t>
-  </si>
-  <si>
-    <t>Il peut décider de supprimer le chapitre.</t>
-  </si>
-  <si>
-    <t>L'affichage de l'éditeur et de son contenu doit se faire en moins de 5 secondes.</t>
-  </si>
-  <si>
     <t>Il récapitule les informations dans un message qui est envoyé par mail à l'administrateur</t>
   </si>
   <si>
     <t>Il affiche à l'utilisateur un message pour lui signaler que l'enregistrement a rencontré un problème.</t>
   </si>
   <si>
-    <t>Il entre du contenu mis en forme dans les champs 'titre' et dans le bloc 'contenu'.</t>
-  </si>
-  <si>
     <t>6.</t>
   </si>
   <si>
-    <t>Il rend le bouton 'valider' cliquable.</t>
-  </si>
-  <si>
-    <t>Scénario nominal : aux points 2 et 4, sur décision de l'utilisateur.</t>
-  </si>
-  <si>
-    <t>4.a</t>
-  </si>
-  <si>
     <t>4.b.</t>
   </si>
   <si>
@@ -215,12 +170,6 @@
     <t>4.c.</t>
   </si>
   <si>
-    <t>Il édite le contenu mis en forme dans les champs 'titre' et dans le bloc 'contenu'.</t>
-  </si>
-  <si>
-    <t>Le chapitre est enregistré en BDD avec son titre, son contenu et la date de publication.</t>
-  </si>
-  <si>
     <t>Fiche descriptive du cas d'utilisation "Add a chapter"</t>
   </si>
   <si>
@@ -230,9 +179,6 @@
     <t>L'utilisateur doit être authentifié en tant qu'auteur ou administrateur, et le chapitre à éditer doit exister en BDD.</t>
   </si>
   <si>
-    <t>L'utilisateur a demandé la page 'editChapter' du chapitre x qu'il souhaite éditer, où x est l'id déjà existant.</t>
-  </si>
-  <si>
     <t>Edit a chapter (package "book editing management")</t>
   </si>
   <si>
@@ -251,38 +197,15 @@
     <t>Exception E1 : après point 6, l'enregistrement du chapitre n'a pas réussi</t>
   </si>
   <si>
-    <t>5.a</t>
-  </si>
-  <si>
     <t>5.b.</t>
   </si>
   <si>
-    <t>Toutes les deux minutes, il enregistre le contenu du bloc 'chapterContent' dans un cookie (il en créé un s'il n'y en a pas encore).</t>
-  </si>
-  <si>
-    <t>Il valide la suppression du chapitre.</t>
-  </si>
-  <si>
     <t>Il envoie la requête au serveur pour supprimer le chapitre de la BDD.</t>
   </si>
   <si>
     <t>Il retourne à l'utilisateur un message pour lui signaler que la suppression s'est bien passé.</t>
   </si>
   <si>
-    <t>Il réaffiche la page active.</t>
-  </si>
-  <si>
-    <t>Il peut décider de ne pas supprimer le chapitre.</t>
-  </si>
-  <si>
-    <t>L'utilisateur doit être authentifié en tant qu'auteur ou administrateur, et le chapitre à éditer doit exister en BDD (s'il demande la suppression à partir de la page d'édition).</t>
-  </si>
-  <si>
-    <t>L'utilisateur a demandé la page 'editChapter' du chapitre x qu'il souhaite éditer, où x est l'id déjà existant.
-Ou
-L'utilisateur a demandé la page 'dashboard'.</t>
-  </si>
-  <si>
     <t>Il demande confirmation à l'utilisateur qu'il souhaite bien supprimer le chapitre.</t>
   </si>
   <si>
@@ -295,13 +218,124 @@
     <t>2.a.</t>
   </si>
   <si>
-    <t>Il peut décider de ne pas confirmer la suppression du chapitre.</t>
-  </si>
-  <si>
     <t>Exception E1 : après point 4, la suppression du chapitre n'a pas réussi</t>
   </si>
   <si>
     <t>Il affiche à l'utilisateur un message pour lui signaler que la suppression a rencontré un problème.</t>
+  </si>
+  <si>
+    <t>Toutes les deux minutes, il enregistre le contenu du bloc 'chapterContent' dans un cookie (il en créé un s'il n'y en existe pas encore).</t>
+  </si>
+  <si>
+    <t>Il envoie la requête au serveur pour enregistrer le contenu en BDD avec le statut 'published'.</t>
+  </si>
+  <si>
+    <t>5.c.</t>
+  </si>
+  <si>
+    <t>5.a.</t>
+  </si>
+  <si>
+    <t>Scénario nominal : aux points 2 et 5, sur décision de l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Le chapitre est enregistré en BDD avec son titre, son contenu, sa date de dernière édition et son statut.</t>
+  </si>
+  <si>
+    <t>Il peut décider de ne pas enregistrer ni publier son travail.</t>
+  </si>
+  <si>
+    <t>L'affichage de la page et de son contenu doit se faire en moins de 5 secondes.</t>
+  </si>
+  <si>
+    <t>1 (version 2)</t>
+  </si>
+  <si>
+    <t>Il envoie une requête à la BDD pour récupérer le contenu du chapitre demandé.</t>
+  </si>
+  <si>
+    <t>Il édite le contenu mis en forme dans les champs 'titre' et dans le bloc d'édition 'contenu'.</t>
+  </si>
+  <si>
+    <t>Il affiche le titre dans l'encart 'title' et le contenu du chapitre déjà enregistré dans le bloc d'édition 'chapter'.</t>
+  </si>
+  <si>
+    <t>Il entre du contenu mis en forme dans les champs 'titre' et dans le bloc d'édition 'contenu'.</t>
+  </si>
+  <si>
+    <t>Il réaffiche le contenu enregistré précédemment dans le bloc d'édition (retour à l'étape 3).</t>
+  </si>
+  <si>
+    <t>2 (version 2)</t>
+  </si>
+  <si>
+    <t>3.a.</t>
+  </si>
+  <si>
+    <t>3.b.</t>
+  </si>
+  <si>
+    <t>Il peut décider d'enregistrer le contenu sans le publier à l'aide du bouton "Valider l'édition" (s'il décide que le chapitre n'est pas prêt pour publication) : le chapitre prendra alors le statut 'saved' en BDD.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>Il peut décider de ne pas entrer de contenu.</t>
+  </si>
+  <si>
+    <t>Scénario nominal : aux points 3 et 6, sur décision de l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Il rend les boutons 'enregistrer le chapitre' et 'publier le chapitre' cliquables si tous les champs sont remplis.</t>
+  </si>
+  <si>
+    <t>Il valide la publication du chapitre avec le bouton 'publier le chapitre'.</t>
+  </si>
+  <si>
+    <t>L'utilisateur a demandé la page 'editChapter' du chapitre qu'il souhaite éditer.</t>
+  </si>
+  <si>
+    <t>L'utilisateur a demandé la page 'newChapter' en dessous de la liste des chapitres déjà existants sur la page 'dashboard'.</t>
+  </si>
+  <si>
+    <t>3 (version 2)</t>
+  </si>
+  <si>
+    <t>25/07/2018 (dernier version : 04/08/2018)</t>
+  </si>
+  <si>
+    <t>20/07/2018 (dernière version : 04/08/2018)</t>
+  </si>
+  <si>
+    <t>19/07/2018 (dernière version : 04/08/2018)</t>
+  </si>
+  <si>
+    <t>L'utilisateur a cliqué sur le bouton 'supprimer le chapitre' sur le tableau de bord (dashboard).</t>
+  </si>
+  <si>
+    <t>Il affiche la page 'dashboard'.</t>
+  </si>
+  <si>
+    <t>Il peut décider de quitter la consultation de la page.</t>
+  </si>
+  <si>
+    <t>Il peut décider de ne pas confirmer la suppression du chapitre (le système réaffichera le bouton 'supprimer le chapitre').</t>
+  </si>
+  <si>
+    <t>Il réaffiche la page 'dashboard'.</t>
+  </si>
+  <si>
+    <t>Reprise au point 3.</t>
+  </si>
+  <si>
+    <t>Scénario nominal : au point 2, sur décision de l'utilisateur.</t>
+  </si>
+  <si>
+    <t>Le chapitre est supprimé de la BDD.</t>
+  </si>
+  <si>
+    <t>La suppression du chapitre et le réaffichage de la page doit se faire en moins de 5 secondes.</t>
   </si>
 </sst>
 </file>
@@ -746,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -868,7 +902,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -912,29 +945,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1259,7 +1292,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28376F6A-11B2-4237-A5FD-AF9AD4AA7569}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1273,89 +1306,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
+      <c r="A1" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
       <c r="B2" s="21"/>
-      <c r="C2" s="55"/>
+      <c r="C2" s="54"/>
       <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="64">
-        <v>1</v>
-      </c>
-      <c r="C3" s="64"/>
+      <c r="B3" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="65"/>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="66"/>
+      <c r="B6" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="64"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="63">
-        <v>43300</v>
-      </c>
-      <c r="C8" s="63"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="67"/>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="67" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="67"/>
+      <c r="B9" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="62"/>
+      <c r="B10" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="66"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
@@ -1370,17 +1403,17 @@
       <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
-      <c r="B14" s="54"/>
+      <c r="B14" s="53"/>
       <c r="C14" s="28"/>
-      <c r="E14" s="53"/>
+      <c r="E14" s="52"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -1399,7 +1432,7 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1407,62 +1440,62 @@
         <v>8</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C17" s="10"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
-        <v>50</v>
+      <c r="A21" s="47" t="s">
+        <v>38</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
-        <v>72</v>
+      <c r="A23" s="47" t="s">
+        <v>54</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,11 +1510,11 @@
       <c r="C25" s="25"/>
     </row>
     <row r="26" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="61" t="s">
+      <c r="A26" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="62"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="27"/>
@@ -1505,7 +1538,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C29" s="8"/>
     </row>
@@ -1514,180 +1547,180 @@
         <v>21</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C30" s="11"/>
     </row>
     <row r="31" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="10"/>
+    </row>
+    <row r="33" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="50"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="57"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="48"/>
+      <c r="D35" s="37"/>
+    </row>
+    <row r="36" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="65"/>
+      <c r="C36" s="65"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="30"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="28"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="51"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="37"/>
-    </row>
-    <row r="35" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="68"/>
-      <c r="C35" s="68"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="28"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="59"/>
-      <c r="D41" s="37"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="60"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="51"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="37"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="59"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="37"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="64"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="B44" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="63"/>
+    </row>
+    <row r="45" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C44" s="66"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="22"/>
-    </row>
-    <row r="47" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="61" t="s">
+      <c r="B45" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="64"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="35"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="22"/>
+    </row>
+    <row r="48" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-    </row>
-    <row r="48" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="33"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="32"/>
-    </row>
-    <row r="49" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="62"/>
+    </row>
+    <row r="49" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="33"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="32"/>
+    </row>
+    <row r="50" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="67" t="s">
+      <c r="B50" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="67"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="C50" s="60"/>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="65" t="s">
+      <c r="B51" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="61"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="65"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51" s="67"/>
+      <c r="B52" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="60"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B8:C8"/>
@@ -1697,6 +1730,15 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1705,7 +1747,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF14559D-95AF-4239-A028-857523A81A71}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1719,88 +1761,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71"/>
+      <c r="A1" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="64">
-        <v>2</v>
-      </c>
-      <c r="C3" s="64"/>
+      <c r="B3" s="63" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="65"/>
+      <c r="B4" s="61" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="66"/>
+      <c r="B6" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="64"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="63">
-        <v>43301</v>
-      </c>
-      <c r="C8" s="63"/>
+      <c r="B8" s="67" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="67"/>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="67"/>
-    </row>
-    <row r="10" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="60"/>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="62"/>
+      <c r="B10" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="66"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
@@ -1808,16 +1850,16 @@
       <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
@@ -1841,301 +1883,307 @@
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="44"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-    </row>
-    <row r="26" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="44"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="C31" s="11"/>
+    </row>
+    <row r="32" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="106.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+    </row>
+    <row r="37" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="44"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="8" t="s">
+    <row r="40" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="37"/>
+    </row>
+    <row r="41" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="10"/>
-    </row>
-    <row r="33" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-    </row>
-    <row r="36" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-    </row>
-    <row r="38" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="37"/>
-    </row>
-    <row r="40" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="50"/>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="49"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="37"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="37"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="64"/>
-    </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="63"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C45" s="66"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="37"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="50"/>
-    </row>
-    <row r="48" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="61" t="s">
+      <c r="B46" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="64"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="37"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="49"/>
+    </row>
+    <row r="49" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="61"/>
-      <c r="C48" s="61"/>
-    </row>
-    <row r="49" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="47"/>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-    </row>
-    <row r="50" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="B49" s="62"/>
+      <c r="C49" s="62"/>
+    </row>
+    <row r="50" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="46"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+    </row>
+    <row r="51" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="67" t="s">
+      <c r="B51" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="C50" s="67"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="C51" s="60"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B51" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="C51" s="66"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B52" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="C52" s="67"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="38"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
+      <c r="B52" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="61"/>
+    </row>
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B53" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="60"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="38"/>
+      <c r="B54" s="39"/>
+      <c r="C54" s="40"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="B44:C44"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -2146,7 +2194,12 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2155,7 +2208,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D21215-922F-4B87-8AE1-D1AC4F8E0C62}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2169,88 +2222,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="71"/>
+      <c r="A1" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="69"/>
+      <c r="C1" s="70"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="64">
-        <v>3</v>
-      </c>
-      <c r="C3" s="64"/>
+      <c r="B3" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="65"/>
+      <c r="B4" s="61" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="61"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="67"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="66" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="66"/>
+      <c r="B6" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="64"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="67"/>
+      <c r="C7" s="60"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="63">
-        <v>43306</v>
-      </c>
-      <c r="C8" s="63"/>
+      <c r="B8" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="67"/>
     </row>
     <row r="9" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="67"/>
+      <c r="B9" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C10" s="62"/>
+      <c r="B10" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="66"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
@@ -2258,16 +2311,16 @@
       <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
@@ -2286,292 +2339,265 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="8"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11" t="s">
-        <v>84</v>
-      </c>
+      <c r="B17" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="8"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-    </row>
-    <row r="24" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="61" t="s">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="37"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="44"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+      <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C25" s="6" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="26" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
     <row r="27" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="45" t="s">
+      <c r="A27" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="11"/>
-    </row>
-    <row r="29" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="11"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="37"/>
-    </row>
-    <row r="33" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="44"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-    </row>
-    <row r="35" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="B27" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+    </row>
+    <row r="30" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="44"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+    </row>
+    <row r="32" spans="1:3" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C32" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="37"/>
-    </row>
-    <row r="37" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12" t="s">
-        <v>90</v>
-      </c>
+    <row r="33" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="37"/>
+    </row>
+    <row r="34" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="37"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="49"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="37"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="50"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
+      <c r="A38" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="63"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="C39" s="64"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B41" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="C41" s="64"/>
-    </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" s="66"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="49"/>
+    </row>
+    <row r="42" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="62"/>
+      <c r="C42" s="62"/>
+    </row>
+    <row r="43" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="46"/>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="37"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="50"/>
-    </row>
-    <row r="45" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="61" t="s">
-        <v>24</v>
-      </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-    </row>
-    <row r="46" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="47"/>
-      <c r="B46" s="47"/>
-      <c r="C46" s="47"/>
-    </row>
-    <row r="47" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A44" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B47" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="67"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
+      <c r="B44" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="60"/>
+    </row>
+    <row r="45" spans="1:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B48" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" s="66"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B49" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="C49" s="67"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="38"/>
-      <c r="B50" s="39"/>
-      <c r="C50" s="40"/>
+      <c r="B45" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="64"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="60"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="40"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>